<commit_message>
lme complete and ccg 1 extra quarter
</commit_message>
<xml_diff>
--- a/data/full_data/ccg.xlsx
+++ b/data/full_data/ccg.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>CCP</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Q1-2017</t>
+  </si>
+  <si>
+    <t>Q3-2016</t>
   </si>
   <si>
     <t>Q2-2017</t>
@@ -483,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC29"/>
+  <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2187,71 +2190,71 @@
         <v>30</v>
       </c>
       <c r="E22" t="n">
-        <v>5417882.97</v>
+        <v>3276799.54</v>
       </c>
       <c r="F22" t="s"/>
       <c r="G22" t="s"/>
       <c r="H22" t="n">
-        <v>1802448000</v>
+        <v>1002954000</v>
       </c>
       <c r="I22" t="n">
-        <v>1802448000</v>
+        <v>1002954000</v>
       </c>
       <c r="J22" t="s"/>
       <c r="K22" t="n">
-        <v>5417882.97</v>
+        <v>3276799.54</v>
       </c>
       <c r="L22" t="n">
-        <v>2703672000</v>
+        <v>1002954000</v>
       </c>
       <c r="M22" t="n">
-        <v>1802448000</v>
+        <v>1002954000</v>
       </c>
       <c r="N22" t="s"/>
       <c r="O22" t="n">
-        <v>1254031199</v>
+        <v>1375410255</v>
       </c>
       <c r="P22" t="n">
-        <v>567611984</v>
+        <v>728102072</v>
       </c>
       <c r="Q22" t="n">
-        <v>1623302406.65</v>
+        <v>2346630813.52</v>
       </c>
       <c r="R22" t="n">
-        <v>2347411273.74</v>
+        <v>3246139953.67</v>
       </c>
       <c r="S22" t="n">
-        <v>3136614890.72</v>
+        <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>3102554609.24</v>
+        <v>0</v>
       </c>
       <c r="U22" t="n">
         <v>30</v>
       </c>
       <c r="V22" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="W22" t="n">
         <v>0</v>
       </c>
       <c r="X22" t="n">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="Y22" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Z22" t="n">
         <v>0</v>
       </c>
       <c r="AA22" t="n">
-        <v>75115072580</v>
+        <v>69413628787</v>
       </c>
       <c r="AB22" t="n">
         <v>0</v>
       </c>
       <c r="AC22" t="n">
-        <v>28117183880</v>
+        <v>25443022185</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -2268,71 +2271,71 @@
         <v>31</v>
       </c>
       <c r="E23" t="n">
-        <v>13222922.53</v>
+        <v>12748795.24</v>
       </c>
       <c r="F23" t="s"/>
       <c r="G23" t="s"/>
       <c r="H23" t="n">
-        <v>4399067000</v>
+        <v>3902117000</v>
       </c>
       <c r="I23" t="n">
-        <v>4399067000</v>
+        <v>3902117000</v>
       </c>
       <c r="J23" t="s"/>
       <c r="K23" t="n">
-        <v>13222922.53</v>
+        <v>12748795.24</v>
       </c>
       <c r="L23" t="n">
-        <v>6598600500</v>
+        <v>3902117000</v>
       </c>
       <c r="M23" t="n">
-        <v>4399067000</v>
+        <v>3902117000</v>
       </c>
       <c r="N23" t="s"/>
       <c r="O23" t="n">
-        <v>3343743355</v>
+        <v>2498434108</v>
       </c>
       <c r="P23" t="n">
-        <v>1880087101</v>
+        <v>1468026740</v>
       </c>
       <c r="Q23" t="n">
-        <v>166118480.76</v>
+        <v>296471386.97</v>
       </c>
       <c r="R23" t="n">
-        <v>9147125789.540001</v>
+        <v>5832388330.5</v>
       </c>
       <c r="S23" t="n">
-        <v>7655243900.22</v>
+        <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>7572116142.72</v>
+        <v>0</v>
       </c>
       <c r="U23" t="n">
         <v>17</v>
       </c>
       <c r="V23" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="W23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Y23" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z23" t="n">
         <v>0</v>
       </c>
       <c r="AA23" t="n">
-        <v>1837503922</v>
+        <v>2535772067</v>
       </c>
       <c r="AB23" t="n">
         <v>0</v>
       </c>
       <c r="AC23" t="n">
-        <v>511740559695</v>
+        <v>583142967534</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -2349,44 +2352,44 @@
         <v>32</v>
       </c>
       <c r="E24" t="n">
-        <v>38919.7</v>
+        <v>18028.11</v>
       </c>
       <c r="F24" t="s"/>
       <c r="G24" t="s"/>
       <c r="H24" t="n">
-        <v>12948000</v>
+        <v>5518000</v>
       </c>
       <c r="I24" t="n">
-        <v>12948000</v>
+        <v>5518000</v>
       </c>
       <c r="J24" t="s"/>
       <c r="K24" t="n">
-        <v>38919.7</v>
+        <v>18028.11</v>
       </c>
       <c r="L24" t="n">
-        <v>19422000</v>
+        <v>5518000</v>
       </c>
       <c r="M24" t="n">
-        <v>12948000</v>
+        <v>5518000</v>
       </c>
       <c r="N24" t="s"/>
       <c r="O24" t="n">
-        <v>10150219</v>
+        <v>13067571</v>
       </c>
       <c r="P24" t="n">
-        <v>4012673</v>
+        <v>4531181</v>
       </c>
       <c r="Q24" t="n">
-        <v>10854633.38</v>
+        <v>11681583.51</v>
       </c>
       <c r="R24" t="n">
-        <v>10901185.58</v>
+        <v>11808938.51</v>
       </c>
       <c r="S24" t="n">
-        <v>22532072.83</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>22287398.63</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
         <v>7</v>
@@ -2398,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="Y24" t="n">
         <v>5</v>
@@ -2407,13 +2410,13 @@
         <v>0</v>
       </c>
       <c r="AA24" t="n">
-        <v>6816990863</v>
+        <v>5577396316</v>
       </c>
       <c r="AB24" t="n">
         <v>0</v>
       </c>
       <c r="AC24" t="n">
-        <v>133534968</v>
+        <v>196638647</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -2430,44 +2433,44 @@
         <v>33</v>
       </c>
       <c r="E25" t="n">
-        <v>751.46</v>
+        <v>1241.51</v>
       </c>
       <c r="F25" t="s"/>
       <c r="G25" t="s"/>
       <c r="H25" t="n">
-        <v>250000</v>
+        <v>380000</v>
       </c>
       <c r="I25" t="n">
-        <v>250000</v>
+        <v>380000</v>
       </c>
       <c r="J25" t="s"/>
       <c r="K25" t="n">
-        <v>751.46</v>
+        <v>1241.51</v>
       </c>
       <c r="L25" t="n">
-        <v>375000</v>
+        <v>380000</v>
       </c>
       <c r="M25" t="n">
-        <v>250000</v>
+        <v>380000</v>
       </c>
       <c r="N25" t="s"/>
       <c r="O25" t="n">
-        <v>265437</v>
+        <v>1028000</v>
       </c>
       <c r="P25" t="n">
-        <v>68884</v>
+        <v>570071</v>
       </c>
       <c r="Q25" t="n">
-        <v>190023.72</v>
+        <v>292487.99</v>
       </c>
       <c r="R25" t="n">
-        <v>190023.72</v>
+        <v>312794.98</v>
       </c>
       <c r="S25" t="n">
-        <v>435049.29</v>
+        <v>0</v>
       </c>
       <c r="T25" t="n">
-        <v>430325.12</v>
+        <v>0</v>
       </c>
       <c r="U25" t="n">
         <v>3</v>
@@ -2482,19 +2485,19 @@
         <v>2</v>
       </c>
       <c r="Y25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
       </c>
       <c r="AA25" t="n">
-        <v>994152</v>
+        <v>2466796</v>
       </c>
       <c r="AB25" t="n">
         <v>0</v>
       </c>
       <c r="AC25" t="n">
-        <v>1206500</v>
+        <v>2979000</v>
       </c>
     </row>
     <row r="26" spans="1:29">
@@ -2511,71 +2514,71 @@
         <v>30</v>
       </c>
       <c r="E26" t="n">
-        <v>6297295</v>
+        <v>5417882.97</v>
       </c>
       <c r="F26" t="s"/>
       <c r="G26" t="s"/>
       <c r="H26" t="n">
-        <v>2103507000</v>
+        <v>1802448000</v>
       </c>
       <c r="I26" t="n">
-        <v>2103507000</v>
+        <v>1802448000</v>
       </c>
       <c r="J26" t="s"/>
       <c r="K26" t="n">
-        <v>6297295</v>
+        <v>5417882.97</v>
       </c>
       <c r="L26" t="n">
-        <v>3155260500</v>
+        <v>2703672000</v>
       </c>
       <c r="M26" t="n">
-        <v>2103507000</v>
+        <v>1802448000</v>
       </c>
       <c r="N26" t="s"/>
       <c r="O26" t="n">
-        <v>1623357537</v>
+        <v>1254031199</v>
       </c>
       <c r="P26" t="n">
-        <v>623862187</v>
+        <v>567611984</v>
       </c>
       <c r="Q26" t="n">
-        <v>1729419191.77</v>
+        <v>1623302406.65</v>
       </c>
       <c r="R26" t="n">
-        <v>2264452704.68</v>
+        <v>2347411273.74</v>
       </c>
       <c r="S26" t="n">
-        <v>2535803818.47</v>
+        <v>3136614890.72</v>
       </c>
       <c r="T26" t="n">
-        <v>2492438137.62</v>
+        <v>3102554609.24</v>
       </c>
       <c r="U26" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V26" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="W26" t="n">
         <v>0</v>
       </c>
       <c r="X26" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="Y26" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z26" t="n">
         <v>0</v>
       </c>
       <c r="AA26" t="n">
-        <v>81244412698</v>
+        <v>75115072580</v>
       </c>
       <c r="AB26" t="n">
         <v>0</v>
       </c>
       <c r="AC26" t="n">
-        <v>27248545597</v>
+        <v>28117183880</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -2592,56 +2595,56 @@
         <v>31</v>
       </c>
       <c r="E27" t="n">
-        <v>12877592</v>
+        <v>13222922.53</v>
       </c>
       <c r="F27" t="s"/>
       <c r="G27" t="s"/>
       <c r="H27" t="n">
-        <v>4301551000</v>
+        <v>4399067000</v>
       </c>
       <c r="I27" t="n">
-        <v>4301551000</v>
+        <v>4399067000</v>
       </c>
       <c r="J27" t="s"/>
       <c r="K27" t="n">
-        <v>12877592</v>
+        <v>13222922.53</v>
       </c>
       <c r="L27" t="n">
-        <v>6452326500</v>
+        <v>6598600500</v>
       </c>
       <c r="M27" t="n">
-        <v>4301551000</v>
+        <v>4399067000</v>
       </c>
       <c r="N27" t="s"/>
       <c r="O27" t="n">
-        <v>3273633809</v>
+        <v>3343743355</v>
       </c>
       <c r="P27" t="n">
-        <v>1687997522</v>
+        <v>1880087101</v>
       </c>
       <c r="Q27" t="n">
-        <v>338879022.72</v>
+        <v>166118480.76</v>
       </c>
       <c r="R27" t="n">
-        <v>8925595799.9</v>
+        <v>9147125789.540001</v>
       </c>
       <c r="S27" t="n">
-        <v>5185573164.79</v>
+        <v>7655243900.22</v>
       </c>
       <c r="T27" t="n">
-        <v>5096892838.16</v>
+        <v>7572116142.72</v>
       </c>
       <c r="U27" t="n">
         <v>17</v>
       </c>
       <c r="V27" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="W27" t="n">
         <v>0</v>
       </c>
       <c r="X27" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y27" t="n">
         <v>10</v>
@@ -2650,13 +2653,13 @@
         <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>1474852443</v>
+        <v>1837503922</v>
       </c>
       <c r="AB27" t="n">
         <v>0</v>
       </c>
       <c r="AC27" t="n">
-        <v>580354322053</v>
+        <v>511740559695</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -2673,47 +2676,47 @@
         <v>32</v>
       </c>
       <c r="E28" t="n">
-        <v>8674</v>
+        <v>38919.7</v>
       </c>
       <c r="F28" t="s"/>
       <c r="G28" t="s"/>
       <c r="H28" t="n">
-        <v>2899000</v>
+        <v>12948000</v>
       </c>
       <c r="I28" t="n">
-        <v>2899000</v>
+        <v>12948000</v>
       </c>
       <c r="J28" t="s"/>
       <c r="K28" t="n">
-        <v>8674</v>
+        <v>38919.7</v>
       </c>
       <c r="L28" t="n">
-        <v>4348500</v>
+        <v>19422000</v>
       </c>
       <c r="M28" t="n">
-        <v>2899000</v>
+        <v>12948000</v>
       </c>
       <c r="N28" t="s"/>
       <c r="O28" t="n">
-        <v>9328880</v>
+        <v>10150219</v>
       </c>
       <c r="P28" t="n">
-        <v>2740661</v>
+        <v>4012673</v>
       </c>
       <c r="Q28" t="n">
-        <v>1843043.55</v>
+        <v>10854633.38</v>
       </c>
       <c r="R28" t="n">
-        <v>1843043.55</v>
+        <v>10901185.58</v>
       </c>
       <c r="S28" t="n">
-        <v>3494780.51</v>
+        <v>22532072.83</v>
       </c>
       <c r="T28" t="n">
-        <v>3435015.03</v>
+        <v>22287398.63</v>
       </c>
       <c r="U28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V28" t="n">
         <v>0</v>
@@ -2722,22 +2725,22 @@
         <v>0</v>
       </c>
       <c r="X28" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Y28" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z28" t="n">
         <v>0</v>
       </c>
       <c r="AA28" t="n">
-        <v>8052868016</v>
+        <v>6816990863</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
       <c r="AC28" t="n">
-        <v>27299396</v>
+        <v>133534968</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -2754,44 +2757,44 @@
         <v>33</v>
       </c>
       <c r="E29" t="n">
-        <v>602</v>
+        <v>751.46</v>
       </c>
       <c r="F29" t="s"/>
       <c r="G29" t="s"/>
       <c r="H29" t="n">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="I29" t="n">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="J29" t="s"/>
       <c r="K29" t="n">
-        <v>602</v>
+        <v>751.46</v>
       </c>
       <c r="L29" t="n">
-        <v>300000</v>
+        <v>375000</v>
       </c>
       <c r="M29" t="n">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="N29" t="s"/>
       <c r="O29" t="n">
-        <v>122444</v>
+        <v>265437</v>
       </c>
       <c r="P29" t="n">
-        <v>10122</v>
+        <v>68884</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>190023.72</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>190023.72</v>
       </c>
       <c r="S29" t="n">
-        <v>241102.48</v>
+        <v>435049.29</v>
       </c>
       <c r="T29" t="n">
-        <v>236979.31</v>
+        <v>430325.12</v>
       </c>
       <c r="U29" t="n">
         <v>3</v>
@@ -2803,21 +2806,345 @@
         <v>0</v>
       </c>
       <c r="X29" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>994152</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>1206500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="n">
+        <v>6297295</v>
+      </c>
+      <c r="F30" t="s"/>
+      <c r="G30" t="s"/>
+      <c r="H30" t="n">
+        <v>2103507000</v>
+      </c>
+      <c r="I30" t="n">
+        <v>2103507000</v>
+      </c>
+      <c r="J30" t="s"/>
+      <c r="K30" t="n">
+        <v>6297295</v>
+      </c>
+      <c r="L30" t="n">
+        <v>3155260500</v>
+      </c>
+      <c r="M30" t="n">
+        <v>2103507000</v>
+      </c>
+      <c r="N30" t="s"/>
+      <c r="O30" t="n">
+        <v>1623357537</v>
+      </c>
+      <c r="P30" t="n">
+        <v>623862187</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>1729419191.77</v>
+      </c>
+      <c r="R30" t="n">
+        <v>2264452704.68</v>
+      </c>
+      <c r="S30" t="n">
+        <v>2535803818.47</v>
+      </c>
+      <c r="T30" t="n">
+        <v>2492438137.62</v>
+      </c>
+      <c r="U30" t="n">
+        <v>29</v>
+      </c>
+      <c r="V30" t="n">
+        <v>16</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>62</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>81244412698</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>27248545597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="n">
+        <v>12877592</v>
+      </c>
+      <c r="F31" t="s"/>
+      <c r="G31" t="s"/>
+      <c r="H31" t="n">
+        <v>4301551000</v>
+      </c>
+      <c r="I31" t="n">
+        <v>4301551000</v>
+      </c>
+      <c r="J31" t="s"/>
+      <c r="K31" t="n">
+        <v>12877592</v>
+      </c>
+      <c r="L31" t="n">
+        <v>6452326500</v>
+      </c>
+      <c r="M31" t="n">
+        <v>4301551000</v>
+      </c>
+      <c r="N31" t="s"/>
+      <c r="O31" t="n">
+        <v>3273633809</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1687997522</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>338879022.72</v>
+      </c>
+      <c r="R31" t="n">
+        <v>8925595799.9</v>
+      </c>
+      <c r="S31" t="n">
+        <v>5185573164.79</v>
+      </c>
+      <c r="T31" t="n">
+        <v>5096892838.16</v>
+      </c>
+      <c r="U31" t="n">
+        <v>17</v>
+      </c>
+      <c r="V31" t="n">
+        <v>55</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>1474852443</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>580354322053</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="n">
+        <v>8674</v>
+      </c>
+      <c r="F32" t="s"/>
+      <c r="G32" t="s"/>
+      <c r="H32" t="n">
+        <v>2899000</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2899000</v>
+      </c>
+      <c r="J32" t="s"/>
+      <c r="K32" t="n">
+        <v>8674</v>
+      </c>
+      <c r="L32" t="n">
+        <v>4348500</v>
+      </c>
+      <c r="M32" t="n">
+        <v>2899000</v>
+      </c>
+      <c r="N32" t="s"/>
+      <c r="O32" t="n">
+        <v>9328880</v>
+      </c>
+      <c r="P32" t="n">
+        <v>2740661</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>1843043.55</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1843043.55</v>
+      </c>
+      <c r="S32" t="n">
+        <v>3494780.51</v>
+      </c>
+      <c r="T32" t="n">
+        <v>3435015.03</v>
+      </c>
+      <c r="U32" t="n">
+        <v>6</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>8052868016</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>27299396</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="n">
+        <v>602</v>
+      </c>
+      <c r="F33" t="s"/>
+      <c r="G33" t="s"/>
+      <c r="H33" t="n">
+        <v>200000</v>
+      </c>
+      <c r="I33" t="n">
+        <v>200000</v>
+      </c>
+      <c r="J33" t="s"/>
+      <c r="K33" t="n">
+        <v>602</v>
+      </c>
+      <c r="L33" t="n">
+        <v>300000</v>
+      </c>
+      <c r="M33" t="n">
+        <v>200000</v>
+      </c>
+      <c r="N33" t="s"/>
+      <c r="O33" t="n">
+        <v>122444</v>
+      </c>
+      <c r="P33" t="n">
+        <v>10122</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>241102.48</v>
+      </c>
+      <c r="T33" t="n">
+        <v>236979.31</v>
+      </c>
+      <c r="U33" t="n">
+        <v>3</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
         <v>1</v>
       </c>
-      <c r="Y29" t="n">
+      <c r="Y33" t="n">
         <v>1</v>
       </c>
-      <c r="Z29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA29" t="n">
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
         <v>295374</v>
       </c>
-      <c r="AB29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC29" t="n">
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>